<commit_message>
Fixed script to generate Latitude and Longitude. Generated CSV files of Latitude, Longitude, and Cost of Living. Deleted previous text filse.
</commit_message>
<xml_diff>
--- a/globe/numbeoCoLData/2010CoL.xlsx
+++ b/globe/numbeoCoLData/2010CoL.xlsx
@@ -20,351 +20,696 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
   <si>
     <t xml:space="preserve">Stavanger, Norway</t>
   </si>
   <si>
+    <t xml:space="preserve">Stavanger</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oslo, Norway</t>
   </si>
   <si>
+    <t xml:space="preserve">Oslo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Breda, Netherlands</t>
   </si>
   <si>
+    <t xml:space="preserve">Breda</t>
+  </si>
+  <si>
     <t xml:space="preserve">Copenhagen, Denmark</t>
   </si>
   <si>
+    <t xml:space="preserve">Copenhagen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zurich, Switzerland</t>
   </si>
   <si>
+    <t xml:space="preserve">Zurich</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paris, France</t>
   </si>
   <si>
+    <t xml:space="preserve">Paris</t>
+  </si>
+  <si>
     <t xml:space="preserve">Geneva, Switzerland</t>
   </si>
   <si>
+    <t xml:space="preserve">Geneva</t>
+  </si>
+  <si>
     <t xml:space="preserve">Milan, Italy</t>
   </si>
   <si>
+    <t xml:space="preserve">Milan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dublin, Ireland</t>
   </si>
   <si>
+    <t xml:space="preserve">Dublin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brussels, Belgium</t>
   </si>
   <si>
+    <t xml:space="preserve">Brussels</t>
+  </si>
+  <si>
     <t xml:space="preserve">London, United Kingdom</t>
   </si>
   <si>
+    <t xml:space="preserve">London</t>
+  </si>
+  <si>
     <t xml:space="preserve">Berlin, Germany</t>
   </si>
   <si>
+    <t xml:space="preserve">Berlin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lyon, France</t>
   </si>
   <si>
+    <t xml:space="preserve">Lyon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Helsinki, Finland</t>
   </si>
   <si>
+    <t xml:space="preserve">Helsinki</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tampere, Finland</t>
   </si>
   <si>
+    <t xml:space="preserve">Tampere</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amsterdam, Netherlands</t>
   </si>
   <si>
+    <t xml:space="preserve">Amsterdam</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tarragona, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Tarragona</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stockholm, Sweden</t>
   </si>
   <si>
+    <t xml:space="preserve">Stockholm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oxford, United Kingdom</t>
   </si>
   <si>
+    <t xml:space="preserve">Oxford</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tampa, FL, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Tampa</t>
+  </si>
+  <si>
     <t xml:space="preserve">Munich, Germany</t>
   </si>
   <si>
+    <t xml:space="preserve">Munich</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sydney, Australia</t>
   </si>
   <si>
+    <t xml:space="preserve">Sydney</t>
+  </si>
+  <si>
     <t xml:space="preserve">Columbus, OH, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Columbus</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vienna, Austria</t>
   </si>
   <si>
+    <t xml:space="preserve">Vienna</t>
+  </si>
+  <si>
     <t xml:space="preserve">Madrid, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Madrid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portland, OR, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Portland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atlanta, GA, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Atlanta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Edmonton, Canada</t>
   </si>
   <si>
+    <t xml:space="preserve">Edmonton</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seattle, WA, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Seattle</t>
+  </si>
+  <si>
     <t xml:space="preserve">New York, NY, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">New York</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leeds, United Kingdom</t>
   </si>
   <si>
+    <t xml:space="preserve">Leeds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frankfurt, Germany</t>
   </si>
   <si>
+    <t xml:space="preserve">Frankfurt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barcelona, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Barcelona</t>
+  </si>
+  <si>
     <t xml:space="preserve">Melbourne, Australia</t>
   </si>
   <si>
+    <t xml:space="preserve">Melbourne</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bilbao, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Bilbao</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tel Aviv-yafo, Israel</t>
   </si>
   <si>
+    <t xml:space="preserve">Tel Aviv-yafo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minneapolis, MN, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Minneapolis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Austin, TX, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Austin</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Francisco, CA, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">San Francisco</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tokyo, Japan</t>
   </si>
   <si>
+    <t xml:space="preserve">Tokyo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Boston, MA, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Boston</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seoul, South Korea</t>
   </si>
   <si>
+    <t xml:space="preserve">Seoul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valencia, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Valencia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Philadelphia, PA, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Philadelphia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lisbon, Portugal</t>
   </si>
   <si>
+    <t xml:space="preserve">Lisbon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Balneario Camboriu, Brazil</t>
   </si>
   <si>
+    <t xml:space="preserve">Balneario Camboriu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Montreal, Canada</t>
   </si>
   <si>
+    <t xml:space="preserve">Montreal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valladolid, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Valladolid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toronto, Canada</t>
   </si>
   <si>
+    <t xml:space="preserve">Toronto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abu Dhabi, United Arab Emirates</t>
   </si>
   <si>
+    <t xml:space="preserve">Abu Dhabi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zagreb, Croatia</t>
   </si>
   <si>
+    <t xml:space="preserve">Zagreb</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sevilla, Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Sevilla</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zaragoza (Saragossa), Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">Zaragoza (Saragossa)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lincoln, NE, United States</t>
   </si>
   <si>
+    <t xml:space="preserve">Lincoln</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ljubljana, Slovenia</t>
   </si>
   <si>
+    <t xml:space="preserve">Ljubljana</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nicosia, Cyprus</t>
   </si>
   <si>
+    <t xml:space="preserve">Nicosia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dubai, United Arab Emirates</t>
   </si>
   <si>
+    <t xml:space="preserve">Dubai</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rio De Janeiro, Brazil</t>
   </si>
   <si>
+    <t xml:space="preserve">Rio De Janeiro</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prague, Czech Republic</t>
   </si>
   <si>
+    <t xml:space="preserve">Prague</t>
+  </si>
+  <si>
     <t xml:space="preserve">Athens, Greece</t>
   </si>
   <si>
+    <t xml:space="preserve">Athens</t>
+  </si>
+  <si>
     <t xml:space="preserve">Santiago, Chile</t>
   </si>
   <si>
+    <t xml:space="preserve">Santiago</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tehran, Iran</t>
   </si>
   <si>
+    <t xml:space="preserve">Tehran</t>
+  </si>
+  <si>
     <t xml:space="preserve">Varna, Bulgaria</t>
   </si>
   <si>
+    <t xml:space="preserve">Varna</t>
+  </si>
+  <si>
     <t xml:space="preserve">Riga, Latvia</t>
   </si>
   <si>
+    <t xml:space="preserve">Riga</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hong Kong, Hong Kong</t>
   </si>
   <si>
+    <t xml:space="preserve">Hong Kong</t>
+  </si>
+  <si>
     <t xml:space="preserve">Belgrade, Serbia</t>
   </si>
   <si>
+    <t xml:space="preserve">Belgrade</t>
+  </si>
+  <si>
     <t xml:space="preserve">Miskolc, Hungary</t>
   </si>
   <si>
+    <t xml:space="preserve">Miskolc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Singapore, Singapore</t>
   </si>
   <si>
+    <t xml:space="preserve">Singapore</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amman, Jordan</t>
   </si>
   <si>
+    <t xml:space="preserve">Amman</t>
+  </si>
+  <si>
     <t xml:space="preserve">Budapest, Hungary</t>
   </si>
   <si>
+    <t xml:space="preserve">Budapest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moscow, Russia</t>
   </si>
   <si>
+    <t xml:space="preserve">Moscow</t>
+  </si>
+  <si>
     <t xml:space="preserve">Istanbul, Turkey</t>
   </si>
   <si>
+    <t xml:space="preserve">Istanbul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Budva, Montenegro</t>
   </si>
   <si>
+    <t xml:space="preserve">Budva</t>
+  </si>
+  <si>
     <t xml:space="preserve">Johannesburg, South Africa</t>
   </si>
   <si>
+    <t xml:space="preserve">Johannesburg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gdynia, Poland</t>
   </si>
   <si>
+    <t xml:space="preserve">Gdynia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Novi Sad, Serbia</t>
   </si>
   <si>
+    <t xml:space="preserve">Novi Sad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Medellin, Colombia</t>
   </si>
   <si>
+    <t xml:space="preserve">Medellin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Poznan, Poland</t>
   </si>
   <si>
+    <t xml:space="preserve">Poznan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sofia, Bulgaria</t>
   </si>
   <si>
+    <t xml:space="preserve">Sofia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manama, Bahrain</t>
   </si>
   <si>
+    <t xml:space="preserve">Manama</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bogota, Colombia</t>
   </si>
   <si>
+    <t xml:space="preserve">Bogota</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tirana, Albania</t>
   </si>
   <si>
+    <t xml:space="preserve">Tirana</t>
+  </si>
+  <si>
     <t xml:space="preserve">Warsaw, Poland</t>
   </si>
   <si>
+    <t xml:space="preserve">Warsaw</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asuncion, Paraguay</t>
   </si>
   <si>
+    <t xml:space="preserve">Asuncion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shanghai, China</t>
   </si>
   <si>
+    <t xml:space="preserve">Shanghai</t>
+  </si>
+  <si>
     <t xml:space="preserve">Esfahan, Iran</t>
   </si>
   <si>
+    <t xml:space="preserve">Esfahan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Guadalajara, Mexico</t>
   </si>
   <si>
+    <t xml:space="preserve">Guadalajara</t>
+  </si>
+  <si>
     <t xml:space="preserve">Constanta, Romania</t>
   </si>
   <si>
+    <t xml:space="preserve">Constanta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adana, Turkey</t>
   </si>
   <si>
+    <t xml:space="preserve">Adana</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vilnius, Lithuania</t>
   </si>
   <si>
+    <t xml:space="preserve">Vilnius</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mexico City, Mexico</t>
   </si>
   <si>
+    <t xml:space="preserve">Mexico City</t>
+  </si>
+  <si>
     <t xml:space="preserve">Santa Marta, Colombia</t>
   </si>
   <si>
+    <t xml:space="preserve">Santa Marta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Banja Luka, Bosnia And Herzegovina</t>
   </si>
   <si>
+    <t xml:space="preserve">Banja Luka</t>
+  </si>
+  <si>
     <t xml:space="preserve">Buenos Aires, Argentina</t>
   </si>
   <si>
+    <t xml:space="preserve">Buenos Aires</t>
+  </si>
+  <si>
     <t xml:space="preserve">Perm, Russia</t>
   </si>
   <si>
+    <t xml:space="preserve">Perm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Caracas, Venezuela</t>
   </si>
   <si>
+    <t xml:space="preserve">Caracas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bucharest, Romania</t>
   </si>
   <si>
+    <t xml:space="preserve">Bucharest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Beijing, China</t>
   </si>
   <si>
+    <t xml:space="preserve">Beijing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minsk, Belarus</t>
   </si>
   <si>
+    <t xml:space="preserve">Minsk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cluj-napoca, Romania</t>
   </si>
   <si>
+    <t xml:space="preserve">Cluj-napoca</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jakarta, Indonesia</t>
   </si>
   <si>
+    <t xml:space="preserve">Jakarta</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Paz, Bolivia</t>
   </si>
   <si>
+    <t xml:space="preserve">La Paz</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ahmedabad, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Ahmedabad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kuala Lumpur, Malaysia</t>
   </si>
   <si>
+    <t xml:space="preserve">Kuala Lumpur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bangkok, Thailand</t>
   </si>
   <si>
+    <t xml:space="preserve">Bangkok</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kharkiv, Ukraine</t>
   </si>
   <si>
+    <t xml:space="preserve">Kharkiv</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kolkata, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Kolkata</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dnipropetrovsk, Ukraine</t>
   </si>
   <si>
+    <t xml:space="preserve">Dnipropetrovsk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kiev, Ukraine</t>
   </si>
   <si>
+    <t xml:space="preserve">Kiev</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mumbai, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Mumbai</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pune, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Pune</t>
+  </si>
+  <si>
     <t xml:space="preserve">Delhi, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Delhi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hyderabad, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Hyderabad</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chennai, India</t>
   </si>
   <si>
+    <t xml:space="preserve">Chennai</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bangalore, India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangalore</t>
   </si>
 </sst>
 </file>
@@ -379,6 +724,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -471,15 +817,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,917 +835,1952 @@
       <c r="B1" s="1" t="n">
         <v>169.2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>58.9680427</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5.7324722</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>152.85</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>59.9132694</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>10.7391112</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>139.7</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>51.5644477</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4.75122967849</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>138.91</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>55.6867243</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>12.5700724</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>132.03</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>47.3685586</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>8.5404434</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>130.3</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>48.8566101</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>2.3514992</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>122.69</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>46.2017559</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>6.1466014</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>122.58</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>45.4667971</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>9.1904984</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>120.79</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>53.3497645</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>-6.2602731</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>120</v>
       </c>
+      <c r="D10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>50.8465565</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>4.351697</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>118.47</v>
       </c>
+      <c r="D11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>51.5073219</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>-0.1276473</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>115.24</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>52.5170365</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>13.3888599</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>115.04</v>
       </c>
+      <c r="D13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>45.7578137</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>4.8320114</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>113.91</v>
       </c>
+      <c r="D14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>60.1674086</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>24.9425683</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>111.96</v>
       </c>
+      <c r="D15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>61.4980214</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>23.7603118</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>111.3</v>
       </c>
+      <c r="D16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>52.3745403</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>4.89797550562</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>111.19</v>
       </c>
+      <c r="D17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>41.1172364</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1.2546057</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>111.02</v>
       </c>
+      <c r="D18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>59.3251172</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>18.0710935</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>110.15</v>
       </c>
+      <c r="D19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>51.7520131</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>-1.2578498</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>109.64</v>
       </c>
+      <c r="D20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>27.9477595</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>-82.4584439</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>107.96</v>
       </c>
+      <c r="D21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>48.1371079</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>11.5753822</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>104.83</v>
       </c>
+      <c r="D22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>-33.8679573</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>151.210047</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>104.69</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>39.9622601</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>-83.0007064</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>103.88</v>
       </c>
+      <c r="D24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>48.2083537</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>16.3725042</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>103.67</v>
       </c>
+      <c r="D25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>40.4167047</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>-3.7035824</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>102.9</v>
       </c>
+      <c r="D26" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>45.5202471</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>-122.6741948</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>100.99</v>
       </c>
+      <c r="D27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>33.7490987</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>-84.3901848</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>100.36</v>
       </c>
+      <c r="D28" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>53.5343609</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>-113.5065084</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>100.33</v>
       </c>
+      <c r="D29" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>47.6038321</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>-122.3300623</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="D30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>40.7305991</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>-73.9865811</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>99.5</v>
       </c>
+      <c r="D31" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>53.7974185</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>-1.543794</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>97.86</v>
       </c>
+      <c r="D32" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>50.1106529</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>8.6820934</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>96.82</v>
       </c>
+      <c r="D33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>41.3825596</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>2.1771353</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>96.36</v>
       </c>
+      <c r="D34" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>-37.8142175</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>144.9631608</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>96.04</v>
       </c>
+      <c r="D35" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>43.2629489</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>-2.9349458</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>94</v>
       </c>
+      <c r="D36" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>32.0804808</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>34.7805274</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>92.85</v>
       </c>
+      <c r="D37" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>44.9772995</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>-93.2654691</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>91.38</v>
       </c>
+      <c r="D38" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>30.2711286</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>-97.7436994</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>90.64</v>
       </c>
+      <c r="D39" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>37.7792808</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>-122.4192362</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>89.31</v>
       </c>
+      <c r="D40" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>34.2255804</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>139.294774527</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>89.11</v>
       </c>
+      <c r="D41" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>42.3604823</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>-71.0595677</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>88.6</v>
       </c>
+      <c r="D42" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>37.5666791</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>126.9782914</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>86.07</v>
       </c>
+      <c r="D43" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>39.4699014</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>-0.3759512</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>85.45</v>
       </c>
+      <c r="D44" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>39.9523993</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>-75.1635898</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>85.42</v>
       </c>
+      <c r="D45" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>38.7077926</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>-9.136506</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>85.38</v>
       </c>
+      <c r="D46" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>-26.9924394</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>-48.6339781</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>85.34</v>
       </c>
+      <c r="D47" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>45.4971225</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>-73.6114885</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>84.45</v>
       </c>
+      <c r="D48" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>41.7030484</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>-4.69695077904</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>83.37</v>
       </c>
+      <c r="D49" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>43.6529206</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>-79.3849007</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>82.82</v>
       </c>
+      <c r="D50" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>24.4747961</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>54.3705762</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>82.23</v>
       </c>
+      <c r="D51" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>45.8131545</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>15.9770298</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>79.5</v>
       </c>
+      <c r="D52" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>37.3886303</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>-5.995317</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>79.31</v>
       </c>
+      <c r="D53" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>41.6521342</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>-0.8809427</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>79.2</v>
       </c>
+      <c r="D54" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>40.7999998</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>-96.6678212</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>75.99</v>
       </c>
+      <c r="D55" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>46.049865</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>14.5068921</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>75.83</v>
       </c>
+      <c r="D56" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>35.1739302</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>33.364726</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>74.45</v>
       </c>
+      <c r="D57" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>25.2683521</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>55.2961962</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>73.66</v>
       </c>
+      <c r="D58" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>-22.9110136</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>-43.2093726</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>72.08</v>
       </c>
+      <c r="D59" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>50.0874654</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>14.4212503</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>71.36</v>
       </c>
+      <c r="D60" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>39.3292396</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>-82.1012554</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>70.67</v>
       </c>
+      <c r="D61" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>-33.4377967</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>-70.650445</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>69.14</v>
       </c>
+      <c r="D62" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>35.7006177</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>51.401375</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>68.85</v>
       </c>
+      <c r="D63" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>43.2166104</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>27.9017131</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="B64" s="1" t="n">
         <v>68.18</v>
       </c>
+      <c r="D64" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>56.9493977</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>24.1051846</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="B65" s="1" t="n">
         <v>68.02</v>
       </c>
+      <c r="D65" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>22.2793278</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>114.1628131</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>66.8</v>
       </c>
+      <c r="D66" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>44.8178787</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>20.4568089</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>66.76</v>
       </c>
+      <c r="D67" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>48.1031517</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>20.7902158</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="B68" s="1" t="n">
         <v>65.94</v>
       </c>
+      <c r="D68" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>1.2904527</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>103.852038</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="B69" s="1" t="n">
         <v>65.64</v>
       </c>
+      <c r="D69" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>31.9515694</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>35.9239625</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="B70" s="1" t="n">
         <v>63.73</v>
       </c>
+      <c r="D70" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>47.4983815</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>19.0404707</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="B71" s="1" t="n">
         <v>63.28</v>
       </c>
+      <c r="D71" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>55.7506828</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>37.6174976</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1" t="n">
         <v>62.6</v>
       </c>
+      <c r="D72" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>41.0096334</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>28.9651646</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="B73" s="1" t="n">
         <v>61.13</v>
       </c>
+      <c r="D73" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>42.2835454</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>18.8378775</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="B74" s="1" t="n">
         <v>61.11</v>
       </c>
+      <c r="D74" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>-26.2049999</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>28.0497222</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="B75" s="1" t="n">
         <v>60.16</v>
       </c>
+      <c r="D75" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>54.5164982</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>18.5402738</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="B76" s="1" t="n">
         <v>59.65</v>
       </c>
+      <c r="D76" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>45.2551053</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>19.845081</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="B77" s="1" t="n">
         <v>59.16</v>
       </c>
+      <c r="D77" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>6.2443382</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>-75.5735529</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>154</v>
       </c>
       <c r="B78" s="1" t="n">
         <v>56.5</v>
       </c>
+      <c r="D78" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>52.4082663</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>16.9335199</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="B79" s="1" t="n">
         <v>56.08</v>
       </c>
+      <c r="D79" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>42.6977211</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>23.3225964</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="B80" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="D80" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>26.2235041</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>50.5822436</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="B81" s="1" t="n">
         <v>54.36</v>
       </c>
+      <c r="D81" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>4.5980478</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>-74.0760866</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="B82" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="D82" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>41.31588575</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>19.9009121645</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="B83" s="1" t="n">
         <v>53.89</v>
       </c>
+      <c r="D83" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>52.2319237</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>21.0067265</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="B84" s="1" t="n">
         <v>53.59</v>
       </c>
+      <c r="D84" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>-25.2959915</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>-57.6311195</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="B85" s="1" t="n">
         <v>53.2</v>
       </c>
+      <c r="D85" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>31.2253441</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>121.4888922</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="B86" s="1" t="n">
         <v>52.95</v>
       </c>
+      <c r="D86" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>32.6707877</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>51.6650002</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="B87" s="1" t="n">
         <v>50.8</v>
       </c>
+      <c r="D87" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>40.7399963</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>-2.50592992588</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>87</v>
+        <v>174</v>
       </c>
       <c r="B88" s="1" t="n">
         <v>50.73</v>
       </c>
+      <c r="D88" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>44.1724166</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>28.620819663</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="B89" s="1" t="n">
         <v>50.15</v>
       </c>
+      <c r="D89" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>37.0033484</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>35.3263252</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="B90" s="1" t="n">
         <v>50.06</v>
       </c>
+      <c r="D90" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>54.6870458</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>25.2829111</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="B91" s="1" t="n">
         <v>49.39</v>
       </c>
+      <c r="D91" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>19.4326009</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>-99.1333415</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="B92" s="1" t="n">
         <v>49.19</v>
       </c>
+      <c r="D92" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>11.0869172</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>-73.8807027103</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="B93" s="1" t="n">
         <v>48.96</v>
       </c>
+      <c r="D93" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>44.7719893</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>17.1898768</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="B94" s="1" t="n">
         <v>47.15</v>
       </c>
+      <c r="D94" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>-34.6075797</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>-58.4375796</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>94</v>
+        <v>188</v>
       </c>
       <c r="B95" s="1" t="n">
         <v>46.33</v>
       </c>
+      <c r="D95" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>58.0149643</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>56.2467244</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="B96" s="1" t="n">
         <v>43.93</v>
       </c>
+      <c r="D96" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>10.506098</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>-66.9146016</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="B97" s="1" t="n">
         <v>43.73</v>
       </c>
+      <c r="D97" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>44.4361414</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>26.1027202</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="B98" s="1" t="n">
         <v>43.16</v>
       </c>
+      <c r="D98" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>39.9059631</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>116.391248</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>98</v>
+        <v>196</v>
       </c>
       <c r="B99" s="1" t="n">
         <v>43.04</v>
       </c>
+      <c r="D99" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>53.902334</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>27.5618791</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="B100" s="1" t="n">
         <v>42.49</v>
       </c>
+      <c r="D100" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>46.7693367</v>
+      </c>
+      <c r="F100" s="0" t="n">
+        <v>23.5900604</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B101" s="1" t="n">
         <v>40.83</v>
       </c>
+      <c r="D101" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>-6.1753941</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>106.8271826</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="B102" s="1" t="n">
         <v>39.76</v>
       </c>
+      <c r="D102" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>-16.4956405</v>
+      </c>
+      <c r="F102" s="0" t="n">
+        <v>-68.1334547</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>102</v>
+        <v>204</v>
       </c>
       <c r="B103" s="1" t="n">
         <v>38.37</v>
       </c>
+      <c r="D103" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E103" s="0" t="n">
+        <v>23.0216238</v>
+      </c>
+      <c r="F103" s="0" t="n">
+        <v>72.5797068</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="B104" s="1" t="n">
         <v>37.55</v>
       </c>
+      <c r="D104" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="E104" s="0" t="n">
+        <v>2.74378195</v>
+      </c>
+      <c r="F104" s="0" t="n">
+        <v>101.711611883</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="B105" s="1" t="n">
         <v>36.56</v>
       </c>
+      <c r="D105" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>13.7538929</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>100.8160803</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="B106" s="1" t="n">
         <v>35.73</v>
       </c>
+      <c r="D106" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E106" s="0" t="n">
+        <v>49.9902794</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>36.2303893</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>106</v>
+        <v>212</v>
       </c>
       <c r="B107" s="1" t="n">
         <v>34.79</v>
       </c>
+      <c r="D107" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E107" s="0" t="n">
+        <v>22.5677459</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>88.3476023</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>107</v>
+        <v>214</v>
       </c>
       <c r="B108" s="1" t="n">
         <v>33.83</v>
       </c>
+      <c r="D108" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="E108" s="0" t="n">
+        <v>48.4680221</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>35.0417711</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>108</v>
+        <v>216</v>
       </c>
       <c r="B109" s="1" t="n">
         <v>33.76</v>
       </c>
+      <c r="D109" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="E109" s="0" t="n">
+        <v>50.4501071</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <v>30.5240501</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>109</v>
+        <v>218</v>
       </c>
       <c r="B110" s="1" t="n">
         <v>33.26</v>
       </c>
+      <c r="D110" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="E110" s="0" t="n">
+        <v>18.9321862</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>72.8308337</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="B111" s="1" t="n">
         <v>32.55</v>
       </c>
+      <c r="D111" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E111" s="0" t="n">
+        <v>18.64395815</v>
+      </c>
+      <c r="F111" s="0" t="n">
+        <v>73.9325681901</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>111</v>
+        <v>222</v>
       </c>
       <c r="B112" s="1" t="n">
         <v>32.43</v>
       </c>
+      <c r="D112" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E112" s="0" t="n">
+        <v>28.6517178</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>77.2219388</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>112</v>
+        <v>224</v>
       </c>
       <c r="B113" s="1" t="n">
         <v>32</v>
       </c>
+      <c r="D113" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="E113" s="0" t="n">
+        <v>17.3616227</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>78.4747305</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="B114" s="1" t="n">
         <v>31.18</v>
       </c>
+      <c r="D114" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <v>13.0796914</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>80.2829533</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="B115" s="1" t="n">
         <v>29.82</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <v>12.9791198</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>77.5912997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally got the globe to display! All JSON datasets were required to be the same length. Unfortunately this also causes some wonky positioning for years that are not 2016.
</commit_message>
<xml_diff>
--- a/globe/numbeoCoLData/2010CoL.xlsx
+++ b/globe/numbeoCoLData/2010CoL.xlsx
@@ -337,7 +337,7 @@
     <t xml:space="preserve">Zaragoza (Saragossa), Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">Zaragoza (Saragossa)</t>
+    <t xml:space="preserve">Zaragoza</t>
   </si>
   <si>
     <t xml:space="preserve">Lincoln, NE, United States</t>
@@ -819,13 +819,13 @@
   </sheetPr>
   <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F105" activeCellId="0" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>